<commit_message>
updated wing size and body size data
</commit_message>
<xml_diff>
--- a/data/thermal_tolerance.xlsx
+++ b/data/thermal_tolerance.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27510"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\研究生学习资料\AFEC-X 2022 project\mini-project\dung-beetle-thermal-tolerance\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/afec-x/0_miniproject/dung-beetle-thermal-tolerance/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D34EF71-8BA5-486F-A4D1-27B09C266244}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="9600" xr2:uid="{7CF4B03A-193E-40ED-ABCC-D31A6DF11667}"/>
+    <workbookView xWindow="9180" yWindow="500" windowWidth="19620" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,9 +17,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$Q$50</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -135,23 +140,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="176" formatCode="0.0000_ "/>
-    <numFmt numFmtId="177" formatCode="0.0_ "/>
-    <numFmt numFmtId="178" formatCode="0.00_ "/>
+    <numFmt numFmtId="164" formatCode="0.0000_ "/>
+    <numFmt numFmtId="165" formatCode="0.0_ "/>
+    <numFmt numFmtId="166" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -159,20 +164,20 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -197,23 +202,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -524,32 +531,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B20C5B0E-F9F2-44AD-9759-0BE74A9212E3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C51" sqref="A51:XFD55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="2" customWidth="1"/>
-    <col min="4" max="5" width="8.88671875" style="2"/>
-    <col min="6" max="6" width="9.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.5" style="2" customWidth="1"/>
+    <col min="4" max="5" width="8.83203125" style="2"/>
+    <col min="6" max="6" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.21875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="9"/>
-    <col min="11" max="15" width="8.88671875" style="11"/>
-    <col min="16" max="16" width="14.21875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="13.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="14.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.1640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="9"/>
+    <col min="11" max="15" width="8.83203125" style="11"/>
+    <col min="16" max="16" width="14.1640625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="13.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -602,7 +609,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -652,7 +659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>22</v>
       </c>
@@ -702,7 +709,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>22</v>
       </c>
@@ -752,7 +759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -802,7 +809,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -853,7 +860,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -904,7 +911,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -955,7 +962,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1006,7 +1013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1057,7 +1064,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>22</v>
       </c>
@@ -1108,7 +1115,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
@@ -1159,7 +1166,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -1210,7 +1217,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1261,7 +1268,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -1312,7 +1319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -1363,7 +1370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
@@ -1414,7 +1421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1465,7 +1472,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
@@ -1516,7 +1523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -1567,7 +1574,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
@@ -1618,7 +1625,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>22</v>
       </c>
@@ -1669,7 +1676,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1720,7 +1727,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1771,7 +1778,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
@@ -1822,7 +1829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>22</v>
       </c>
@@ -1873,7 +1880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>22</v>
       </c>
@@ -1924,7 +1931,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>22</v>
       </c>
@@ -1975,7 +1982,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
@@ -2026,7 +2033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
@@ -2077,7 +2084,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>22</v>
       </c>
@@ -2128,7 +2135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>22</v>
       </c>
@@ -2179,7 +2186,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>22</v>
       </c>
@@ -2230,7 +2237,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>22</v>
       </c>
@@ -2280,7 +2287,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>22</v>
       </c>
@@ -2330,7 +2337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>22</v>
       </c>
@@ -2380,7 +2387,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>22</v>
       </c>
@@ -2424,7 +2431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>22</v>
       </c>
@@ -2462,7 +2469,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>22</v>
       </c>
@@ -2500,7 +2507,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>22</v>
       </c>
@@ -2538,7 +2545,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
@@ -2576,7 +2583,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>22</v>
       </c>
@@ -2614,7 +2621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>22</v>
       </c>
@@ -2652,7 +2659,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>22</v>
       </c>
@@ -2690,7 +2697,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>22</v>
       </c>
@@ -2728,7 +2735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>22</v>
       </c>
@@ -2766,7 +2773,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>22</v>
       </c>
@@ -2804,7 +2811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>22</v>
       </c>
@@ -2842,7 +2849,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>22</v>
       </c>
@@ -2892,7 +2899,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>22</v>
       </c>
@@ -2942,26 +2949,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B51" s="2" t="s">
+    <row r="51" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C51" s="2">
+      <c r="C51" s="3">
         <v>601</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E51" s="2">
-        <v>50</v>
-      </c>
-      <c r="F51" s="2" t="s">
+      <c r="D51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3">
+        <v>50</v>
+      </c>
+      <c r="F51" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51" s="7">
         <v>0.41689999999999999</v>
       </c>
       <c r="H51" s="7">
@@ -2970,33 +2977,45 @@
       <c r="I51" s="7">
         <v>2.2800000000000001E-2</v>
       </c>
-      <c r="J51" s="9">
+      <c r="J51" s="13">
         <v>43.2</v>
       </c>
-      <c r="K51" s="11">
+      <c r="K51" s="14">
         <v>43.06</v>
       </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B52" s="2" t="s">
+      <c r="L51" s="14">
+        <v>15.92</v>
+      </c>
+      <c r="M51" s="14">
+        <v>8.52</v>
+      </c>
+      <c r="N51" s="14">
+        <v>15.89</v>
+      </c>
+      <c r="O51" s="14">
+        <v>5.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="3">
         <v>602</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E52" s="2">
-        <v>50</v>
-      </c>
-      <c r="F52" s="2" t="s">
+      <c r="D52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>50</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G52" s="7">
         <v>0.34960000000000002</v>
       </c>
       <c r="H52" s="7">
@@ -3005,33 +3024,45 @@
       <c r="I52" s="7">
         <v>2.8899999999999999E-2</v>
       </c>
-      <c r="J52" s="9">
+      <c r="J52" s="13">
         <v>43.9</v>
       </c>
-      <c r="K52" s="11">
+      <c r="K52" s="14">
         <v>43.77</v>
       </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B53" s="2" t="s">
+      <c r="L52" s="14">
+        <v>15.75</v>
+      </c>
+      <c r="M52" s="14">
+        <v>8.83</v>
+      </c>
+      <c r="N52" s="14">
+        <v>15.3</v>
+      </c>
+      <c r="O52" s="14">
+        <v>5.36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="3">
         <v>603</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E53" s="2">
-        <v>50</v>
-      </c>
-      <c r="F53" s="2" t="s">
+      <c r="D53" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53" s="3">
+        <v>50</v>
+      </c>
+      <c r="F53" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G53" s="7">
         <v>0.38740000000000002</v>
       </c>
       <c r="H53" s="7">
@@ -3040,33 +3071,45 @@
       <c r="I53" s="7">
         <v>4.4400000000000002E-2</v>
       </c>
-      <c r="J53" s="9">
+      <c r="J53" s="13">
         <v>46.1</v>
       </c>
-      <c r="K53" s="11">
+      <c r="K53" s="14">
         <v>46.01</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B54" s="2" t="s">
+      <c r="L53" s="14">
+        <v>15.68</v>
+      </c>
+      <c r="M53" s="14">
+        <v>8.7100000000000009</v>
+      </c>
+      <c r="N53" s="14">
+        <v>15.91</v>
+      </c>
+      <c r="O53" s="14">
+        <v>5.19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B54" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="3">
         <v>604</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E54" s="2">
-        <v>50</v>
-      </c>
-      <c r="F54" s="2" t="s">
+      <c r="D54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3">
+        <v>50</v>
+      </c>
+      <c r="F54" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="7">
         <v>0.39900000000000002</v>
       </c>
       <c r="H54" s="7">
@@ -3075,33 +3118,45 @@
       <c r="I54" s="7">
         <v>1.9800000000000002E-2</v>
       </c>
-      <c r="J54" s="9">
+      <c r="J54" s="13">
         <v>46.1</v>
       </c>
-      <c r="K54" s="11">
+      <c r="K54" s="14">
         <v>46.01</v>
       </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B55" s="2" t="s">
+      <c r="L54" s="14">
+        <v>16.04</v>
+      </c>
+      <c r="M54" s="14">
+        <v>8.75</v>
+      </c>
+      <c r="N54" s="14">
+        <v>15.69</v>
+      </c>
+      <c r="O54" s="14">
+        <v>5.61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B55" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="3">
         <v>605</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E55" s="2">
-        <v>50</v>
-      </c>
-      <c r="F55" s="2" t="s">
+      <c r="D55" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3">
+        <v>50</v>
+      </c>
+      <c r="F55" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G55" s="7">
         <v>0.40629999999999999</v>
       </c>
       <c r="H55" s="7">
@@ -3110,14 +3165,26 @@
       <c r="I55" s="7">
         <v>2.92E-2</v>
       </c>
-      <c r="J55" s="9">
+      <c r="J55" s="13">
         <v>45.4</v>
       </c>
-      <c r="K55" s="11">
+      <c r="K55" s="14">
         <v>45.4</v>
       </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="L55" s="14">
+        <v>14.36</v>
+      </c>
+      <c r="M55" s="14">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="N55" s="14">
+        <v>15.35</v>
+      </c>
+      <c r="O55" s="14">
+        <v>5.44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>30</v>
       </c>
@@ -3152,7 +3219,7 @@
         <v>45.69</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>30</v>
       </c>
@@ -3187,7 +3254,7 @@
         <v>45.05</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>30</v>
       </c>
@@ -3222,7 +3289,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>30</v>
       </c>
@@ -3257,7 +3324,7 @@
         <v>44.66</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>30</v>
       </c>
@@ -3292,7 +3359,7 @@
         <v>45.4</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>30</v>
       </c>
@@ -3327,7 +3394,7 @@
         <v>45.69</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>30</v>
       </c>
@@ -3362,7 +3429,7 @@
         <v>45.79</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>30</v>
       </c>
@@ -3397,7 +3464,7 @@
         <v>47.3</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>30</v>
       </c>
@@ -3432,7 +3499,7 @@
         <v>47.08</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>30</v>
       </c>
@@ -3467,7 +3534,7 @@
         <v>46.68</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>30</v>
       </c>
@@ -3502,7 +3569,7 @@
         <v>4.29</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>30</v>
       </c>
@@ -3537,7 +3604,7 @@
         <v>3.82</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>30</v>
       </c>
@@ -3572,7 +3639,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>30</v>
       </c>
@@ -3607,7 +3674,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>30</v>
       </c>
@@ -3642,7 +3709,7 @@
         <v>3.56</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>30</v>
       </c>
@@ -3677,7 +3744,7 @@
         <v>6.73</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>30</v>
       </c>
@@ -3712,7 +3779,7 @@
         <v>7.22</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>30</v>
       </c>
@@ -3747,7 +3814,7 @@
         <v>7.02</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>30</v>
       </c>
@@ -3782,7 +3849,7 @@
         <v>6.73</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>30</v>
       </c>
@@ -3817,7 +3884,7 @@
         <v>6.9</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>30</v>
       </c>
@@ -3852,7 +3919,7 @@
         <v>11.36</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>30</v>
       </c>
@@ -3887,7 +3954,7 @@
         <v>18.190000000000001</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>30</v>
       </c>
@@ -3922,7 +3989,7 @@
         <v>18.190000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>30</v>
       </c>
@@ -3957,7 +4024,7 @@
         <v>14.42</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>
@@ -3992,7 +4059,7 @@
         <v>11.95</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>30</v>
       </c>
@@ -4027,7 +4094,7 @@
         <v>44.2</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>30</v>
       </c>
@@ -4062,7 +4129,7 @@
         <v>43.64</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>30</v>
       </c>
@@ -4097,7 +4164,7 @@
         <v>43.96</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
         <v>30</v>
       </c>
@@ -4132,7 +4199,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>30</v>
       </c>
@@ -4167,7 +4234,7 @@
         <v>43.34</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
         <v>30</v>
       </c>
@@ -4202,7 +4269,7 @@
         <v>45.56</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>30</v>
       </c>
@@ -4237,7 +4304,7 @@
         <v>45.33</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
         <v>30</v>
       </c>
@@ -4272,7 +4339,7 @@
         <v>43.96</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
         <v>30</v>
       </c>
@@ -4307,7 +4374,7 @@
         <v>45.56</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
         <v>30</v>
       </c>
@@ -4330,7 +4397,7 @@
         <v>3.8899999999999997E-2</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
         <v>30</v>
       </c>
@@ -4365,7 +4432,7 @@
         <v>1.37</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
         <v>30</v>
       </c>
@@ -4400,7 +4467,7 @@
         <v>5.23</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
         <v>30</v>
       </c>
@@ -4435,7 +4502,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
         <v>30</v>
       </c>
@@ -4470,7 +4537,7 @@
         <v>1.92</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
         <v>30</v>
       </c>
@@ -4505,7 +4572,7 @@
         <v>1.76</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
         <v>30</v>
       </c>
@@ -4540,7 +4607,7 @@
         <v>10.48</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
         <v>30</v>
       </c>
@@ -4575,7 +4642,7 @@
         <v>3.22</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
         <v>30</v>
       </c>
@@ -4610,7 +4677,7 @@
         <v>5.85</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
         <v>30</v>
       </c>
@@ -4645,7 +4712,7 @@
         <v>3.45</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
         <v>30</v>
       </c>
@@ -4680,7 +4747,7 @@
         <v>6.64</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
         <v>30</v>
       </c>
@@ -4703,7 +4770,7 @@
         <v>0.38059999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
         <v>30</v>
       </c>
@@ -4726,7 +4793,7 @@
         <v>0.40260000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
         <v>30</v>
       </c>
@@ -4749,7 +4816,7 @@
         <v>0.43559999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>30</v>
       </c>
@@ -4772,7 +4839,7 @@
         <v>0.40360000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
         <v>30</v>
       </c>
@@ -4795,7 +4862,7 @@
         <v>0.40039999999999998</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
         <v>30</v>
       </c>
@@ -4818,7 +4885,7 @@
         <v>4.5499999999999999E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
         <v>30</v>
       </c>
@@ -4841,7 +4908,7 @@
         <v>4.1300000000000003E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
         <v>30</v>
       </c>
@@ -4864,7 +4931,7 @@
         <v>5.0799999999999998E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
         <v>30</v>
       </c>
@@ -4887,7 +4954,7 @@
         <v>4.4499999999999998E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>30</v>
       </c>
@@ -4911,7 +4978,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:Q50" xr:uid="{72B916E0-E465-40F4-B2F6-5595672376E8}"/>
+  <autoFilter ref="B1:Q50"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>